<commit_message>
[Fix] Quest data, Quest Script Data 추가
1) 퀘스트 데이터 -  QuestItemID 추가, RewardID 추가
2) 퀘스트 스크립트 데이터 - QuestID , OrderID 제거 => DialogueID 로 변경
</commit_message>
<xml_diff>
--- a/excel2json-master/Quest_Data.xlsx
+++ b/excel2json-master/Quest_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이영선\Desktop\Sparta_Club\Project_P\Project_P\excel2json-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C986B5E-5E0C-4CEB-BC7E-B755E7348A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56FB602-C7C9-40AA-9E7E-F3AE2AC6D8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9585" yWindow="2130" windowWidth="19110" windowHeight="12255" xr2:uid="{3D886221-0E62-48B6-9303-9CD9E684FF2F}"/>
+    <workbookView xWindow="11505" yWindow="1590" windowWidth="16995" windowHeight="13260" xr2:uid="{3D886221-0E62-48B6-9303-9CD9E684FF2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{10F82F32-850D-41D7-8715-1E80663D28DD}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{191E9634-90C1-41D4-832E-AE9975B94046}">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">exp - </t>
+          <t xml:space="preserve">0 - </t>
         </r>
         <r>
           <rPr>
@@ -116,16 +116,39 @@
             <family val="3"/>
             <charset val="129"/>
           </rPr>
-          <t>경험치</t>
-        </r>
-        <r>
-          <rPr>
+          <t>아이템</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">없음
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1 ~ - ItemID
 </t>
         </r>
       </text>
@@ -135,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>QuestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,11 +204,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>exp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>#Quest[{}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestItemID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초급스태미너포션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>샬라리스킬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -231,7 +266,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +276,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,7 +300,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -267,6 +308,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5450F23A-DDCD-4531-84F1-C9A87D28DD5C}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -596,13 +640,16 @@
     <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" customWidth="1"/>
+    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -622,14 +669,20 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1001</v>
       </c>
@@ -648,11 +701,49 @@
       <c r="G2">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2">
-        <v>100</v>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1002</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[fix] Quest Type 데이터 추가
</commit_message>
<xml_diff>
--- a/excel2json-master/Quest_Data.xlsx
+++ b/excel2json-master/Quest_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이영선\Desktop\Sparta_Club\Project_P\Project_P\excel2json-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DB3657-D5AA-4179-B2EA-1F135F0A9693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9E50E6-7608-4E44-9067-10EAF1AB70EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D886221-0E62-48B6-9303-9CD9E684FF2F}"/>
+    <workbookView xWindow="300" yWindow="675" windowWidth="15225" windowHeight="14685" xr2:uid="{3D886221-0E62-48B6-9303-9CD9E684FF2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3737,14 +3737,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5450F23A-DDCD-4531-84F1-C9A87D28DD5C}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="20.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
@@ -3854,6 +3854,9 @@
       <c r="B2">
         <v>1001</v>
       </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
       <c r="D2" t="s">
         <v>31</v>
       </c>
@@ -3919,6 +3922,9 @@
       <c r="B3">
         <v>1002</v>
       </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
       <c r="D3" t="s">
         <v>31</v>
       </c>
@@ -3984,6 +3990,9 @@
       <c r="B4">
         <v>1003</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
       <c r="D4" t="s">
         <v>32</v>
       </c>
@@ -4049,6 +4058,9 @@
       <c r="B5">
         <v>1004</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
       <c r="D5" t="s">
         <v>32</v>
       </c>
@@ -4114,6 +4126,9 @@
       <c r="B6">
         <v>1005</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="D6" t="s">
         <v>32</v>
       </c>
@@ -4182,6 +4197,9 @@
       <c r="B7">
         <v>1006</v>
       </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
       <c r="D7" t="s">
         <v>37</v>
       </c>
@@ -4247,6 +4265,9 @@
       <c r="B8">
         <v>1007</v>
       </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
       <c r="D8" t="s">
         <v>38</v>
       </c>
@@ -4312,6 +4333,9 @@
       <c r="B9">
         <v>1008</v>
       </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
       <c r="D9" t="s">
         <v>39</v>
       </c>
@@ -4377,6 +4401,9 @@
       <c r="B10">
         <v>1009</v>
       </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
       <c r="D10" t="s">
         <v>41</v>
       </c>
@@ -4445,6 +4472,9 @@
       <c r="B11">
         <v>1010</v>
       </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
       <c r="D11" t="s">
         <v>44</v>
       </c>
@@ -4510,6 +4540,9 @@
       <c r="B12">
         <v>1011</v>
       </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
       <c r="D12" t="s">
         <v>45</v>
       </c>
@@ -4578,6 +4611,9 @@
       <c r="B13">
         <v>1012</v>
       </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
       <c r="D13" t="s">
         <v>48</v>
       </c>
@@ -4643,6 +4679,9 @@
       <c r="B14">
         <v>1013</v>
       </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
       <c r="D14" t="s">
         <v>48</v>
       </c>
@@ -4711,6 +4750,9 @@
       <c r="B15">
         <v>1014</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
       <c r="D15" t="s">
         <v>62</v>
       </c>
@@ -4779,6 +4821,9 @@
       <c r="B16">
         <v>1015</v>
       </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
       <c r="D16" t="s">
         <v>62</v>
       </c>
@@ -4844,6 +4889,9 @@
       <c r="B17">
         <v>1016</v>
       </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
       <c r="D17" t="s">
         <v>62</v>
       </c>
@@ -4909,6 +4957,9 @@
       <c r="B18">
         <v>1017</v>
       </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
       <c r="D18" t="s">
         <v>67</v>
       </c>
@@ -4977,6 +5028,9 @@
       <c r="B19">
         <v>1018</v>
       </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
       <c r="D19" t="s">
         <v>67</v>
       </c>
@@ -5045,6 +5099,9 @@
       <c r="B20">
         <v>1019</v>
       </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
       <c r="D20" t="s">
         <v>67</v>
       </c>
@@ -5110,6 +5167,9 @@
       <c r="B21">
         <v>1020</v>
       </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
       <c r="D21" t="s">
         <v>67</v>
       </c>
@@ -5175,6 +5235,9 @@
       <c r="B22">
         <v>1021</v>
       </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
       <c r="D22" t="s">
         <v>67</v>
       </c>
@@ -5240,6 +5303,9 @@
       <c r="B23">
         <v>1022</v>
       </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
       <c r="D23" t="s">
         <v>76</v>
       </c>
@@ -5308,6 +5374,9 @@
       <c r="B24">
         <v>1023</v>
       </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
       <c r="D24" t="s">
         <v>76</v>
       </c>
@@ -5376,6 +5445,9 @@
       <c r="B25">
         <v>1024</v>
       </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
       <c r="D25" t="s">
         <v>79</v>
       </c>
@@ -5444,6 +5516,9 @@
       <c r="B26">
         <v>1025</v>
       </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
       <c r="D26" t="s">
         <v>84</v>
       </c>
@@ -5512,6 +5587,9 @@
       <c r="B27">
         <v>1026</v>
       </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
       <c r="D27" t="s">
         <v>87</v>
       </c>
@@ -5577,6 +5655,9 @@
       <c r="B28">
         <v>1027</v>
       </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
       <c r="D28" t="s">
         <v>92</v>
       </c>
@@ -5645,6 +5726,9 @@
       <c r="B29">
         <v>1028</v>
       </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
       <c r="D29" t="s">
         <v>92</v>
       </c>
@@ -5712,6 +5796,9 @@
     <row r="30" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>1029</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
       </c>
       <c r="D30" t="s">
         <v>92</v>

</xml_diff>